<commit_message>
update the quiz 11.3
</commit_message>
<xml_diff>
--- a/Quizzes/Spectra.xlsx
+++ b/Quizzes/Spectra.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthewrowley1\Desktop\3620\Quizzes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C4393B-BB0D-4158-A2C9-24B1CE0C0EB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F7CF2F-BDB0-4236-8A8C-0210B989BC74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="3" activeTab="4" xr2:uid="{E65C0530-7A76-4299-804D-8365C5750414}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="6" xr2:uid="{E65C0530-7A76-4299-804D-8365C5750414}"/>
   </bookViews>
   <sheets>
     <sheet name="CN Microwave" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="CO Microwave" sheetId="7" r:id="rId4"/>
     <sheet name="CO IR" sheetId="5" r:id="rId5"/>
     <sheet name="CO Raman" sheetId="6" r:id="rId6"/>
+    <sheet name="CO Birge-Sponer" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
   <si>
     <t>J</t>
   </si>
@@ -103,6 +104,117 @@
   <si>
     <t>D1</t>
   </si>
+  <si>
+    <t>J(init)</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>E(cm^-1)</t>
+  </si>
+  <si>
+    <t>μ(AMU)</t>
+  </si>
+  <si>
+    <t>E(J) = B*J*(J+1) - D*J^2*(J+1)^2</t>
+  </si>
+  <si>
+    <t>we</t>
+  </si>
+  <si>
+    <t>wexe</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>v+1/2</t>
+  </si>
+  <si>
+    <t>v+1</t>
+  </si>
+  <si>
+    <t>v + 1/2 line</t>
+  </si>
+  <si>
+    <t>v + 1 line</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>b (νe)</t>
+  </si>
+  <si>
+    <t>x-intercept</t>
+  </si>
+  <si>
+    <t>m (νeχe)</t>
+  </si>
+  <si>
+    <t>J (init)</t>
+  </si>
+  <si>
+    <t>Δν</t>
+  </si>
+  <si>
+    <t>ae</t>
+  </si>
+  <si>
+    <t>Be</t>
+  </si>
+  <si>
+    <t>m(culled)</t>
+  </si>
+  <si>
+    <t>Δν (culled)</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>point1</t>
+  </si>
+  <si>
+    <t>point2</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>intercept</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>mx+b</t>
+  </si>
+  <si>
+    <t>1.9225=-1.23654e-5*1+b</t>
+  </si>
+  <si>
+    <t>y(-0.5)</t>
+  </si>
+  <si>
+    <t>Combination Differences (J=3)</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>αe</t>
+  </si>
+  <si>
+    <t>(νeχe)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (νe)</t>
+  </si>
 </sst>
 </file>
 
@@ -112,7 +224,7 @@
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
     <numFmt numFmtId="165" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,8 +232,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4D5156"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4D5156"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,6 +256,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -147,11 +290,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1479,6 +1628,1030 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CO IR'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Δν</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.46843482064741909"/>
+                  <c:y val="6.7460544704639192E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'CO IR'!$E$2:$E$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'CO IR'!$F$2:$F$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>4.6400000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6089999999999236</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5769999999999982</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.5450000000000728</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.51299999999992</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.4819999999999709</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.4490000000000691</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.4180000000001201</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.3840000000000146</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.3519999999998618</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.3200000000001637</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.2859999999996035</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.2540000000003602</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.2199999999997999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.1869999999998981</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.1530000000002474</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.1199999999998909</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.0859999999997854</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.0520000000001346</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.0180000000000291</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.9830000000001746</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.9490000000000691</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.9149999999999636</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.8799999999996544</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.7750000000000909</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.7390000000000327</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.7049999999999272</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.6680000000001201</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.6329999999998108</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.5970000000002074</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.5599999999999454</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.5249999999996362</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.4880000000002838</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.4519999999997708</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.4160000000001673</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.3780000000001564</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.3419999999996435</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.3040000000000873</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.2670000000002801</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.2300000000000182</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.1929999999997563</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.1550000000002001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.1169999999997344</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.0790000000001783</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.0409999999997126</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.0030000000001564</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.9650000000001455</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.9259999999999309</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.88799999999992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A803-461D-9B0D-FDCBA98BC748}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="516480687"/>
+        <c:axId val="510967919"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="516480687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="510967919"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="510967919"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="516480687"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CO Birge-Sponer'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>E(cm^-1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'CO Birge-Sponer'!$B$2:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'CO Birge-Sponer'!$D$2:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2143.2369600000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2116.6603399999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2090.0837200000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2063.5070999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2036.93048</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2010.3538599999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1983.7772399999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1957.2006200000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1930.624</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1904.04738</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1877.4707600000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1850.8941399999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1824.3175200000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3087-4B7F-8489-AF7F46BD914D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1524452672"/>
+        <c:axId val="1630303776"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1524452672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1630303776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1630303776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1524452672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1599,6 +2772,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2632,6 +3885,1038 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3192,16 +5477,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>119062</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>347662</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>585787</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3228,16 +5513,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>52387</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>204787</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>71436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>442912</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>690562</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>147636</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3257,6 +5542,88 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D48D8DF-5873-4BA3-85EC-286E5FF0192A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EC4F78A-3213-4456-93F2-6151FBEAA1C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3793,10 +6160,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C0820A-18FD-4AE8-BD06-755F0D88AB2E}">
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:M6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3805,9 +6172,10 @@
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3824,7 +6192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3847,7 +6215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3879,8 +6247,14 @@
       <c r="K3">
         <v>1.128323</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3905,8 +6279,24 @@
       <c r="H4" s="2">
         <v>6.1878000000000003E-6</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1.9225000000000001</v>
+      </c>
+      <c r="R4" t="s">
+        <v>50</v>
+      </c>
+      <c r="S4">
+        <f>(P5-P4)/(O5-O4)</f>
+        <v>-1.2364444444444722E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3939,14 +6329,30 @@
         <v>15.994915000000001</v>
       </c>
       <c r="K5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="L5" s="2">
         <f>J5*H5/(J5+H5)</f>
         <v>6.8562087079028471</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5">
+        <v>676</v>
+      </c>
+      <c r="P5">
+        <v>1.9141539999999999</v>
+      </c>
+      <c r="R5" t="s">
+        <v>51</v>
+      </c>
+      <c r="S5">
+        <f>R12</f>
+        <v>1.9225123644444446</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3973,7 +6379,7 @@
         <v>1.1385268528566667E-26</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3995,8 +6401,17 @@
       <c r="G7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="R7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4030,7 +6445,7 @@
         <v>1.1308773665667667E-10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4057,7 +6472,7 @@
         <v>6.184613940156526E-6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4076,8 +6491,11 @@
         <f t="shared" si="2"/>
         <v>1.9215000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="R10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4097,7 +6515,7 @@
         <v>1.9213</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4116,8 +6534,12 @@
         <f t="shared" si="2"/>
         <v>1.9210454545454545</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <f>P4-S4*O4</f>
+        <v>1.9225123644444446</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4137,7 +6559,7 @@
         <v>1.92075</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4157,7 +6579,7 @@
         <v>1.9204230769230768</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4177,7 +6599,7 @@
         <v>1.9201071428571428</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4197,7 +6619,7 @@
         <v>1.9197333333333333</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4217,7 +6639,7 @@
         <v>1.9193750000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -4237,7 +6659,7 @@
         <v>1.9189411764705882</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -4257,7 +6679,7 @@
         <v>1.9185277777777776</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -4277,7 +6699,7 @@
         <v>1.9180526315789472</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -4297,7 +6719,7 @@
         <v>1.917575</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -4317,7 +6739,7 @@
         <v>1.9170714285714285</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -4337,7 +6759,7 @@
         <v>1.9165454545454546</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -4357,7 +6779,7 @@
         <v>1.9159782608695652</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -4377,7 +6799,7 @@
         <v>1.9153958333333332</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -4397,7 +6819,7 @@
         <v>1.9147999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -4417,7 +6839,7 @@
         <v>1.9141538461538461</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -4431,8 +6853,15 @@
         <f>B29*1.3806488E-23/6.626E-34/29980000000</f>
         <v>207.11732280721611</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <f>0.008314*298</f>
+        <v>2.4775719999999999</v>
+      </c>
+      <c r="I29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -4449,7 +6878,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -4470,7 +6899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -5004,496 +7433,1037 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535BBEDA-FF49-4A25-AA6B-6D84D95D0A37}">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>-26</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>2037</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2">
+        <f>-A2</f>
+        <v>-25</v>
+      </c>
+      <c r="F2">
+        <f>B3-B2</f>
+        <v>4.6400000000001</v>
+      </c>
+      <c r="K2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>-25</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>2041.64</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3">
+        <f>-A3</f>
+        <v>-24</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F52" si="0">B4-B3</f>
+        <v>4.6089999999999236</v>
+      </c>
+      <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c r="G3">
+      <c r="L3">
         <f>1.93128-0.5*0.01750441</f>
         <v>1.9225277950000002</v>
       </c>
-      <c r="I3" t="s">
+      <c r="N3" t="s">
         <v>9</v>
       </c>
-      <c r="J3">
+      <c r="O3">
         <v>1.128323</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>-24</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>2046.249</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4">
+        <f>-A4</f>
+        <v>-23</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>4.5769999999999982</v>
+      </c>
+      <c r="K4" t="s">
         <v>21</v>
       </c>
-      <c r="G4">
+      <c r="L4">
         <v>6.1878000000000003E-6</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4">
+        <v>1.7504410000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>-23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>2050.826</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5">
+        <f>-A5</f>
+        <v>-22</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>4.5450000000000728</v>
+      </c>
+      <c r="K5" t="s">
         <v>22</v>
       </c>
-      <c r="G5">
+      <c r="L5">
         <v>1.9050229999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O5">
+        <v>1.9312800000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>-22</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>2055.3710000000001</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6">
+        <f>-A6</f>
+        <v>-21</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>4.51299999999992</v>
+      </c>
+      <c r="K6" t="s">
         <v>23</v>
       </c>
-      <c r="G6">
+      <c r="L6">
         <v>6.1724999999999998E-6</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>-21</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>2059.884</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7">
+        <f>-A7</f>
+        <v>-20</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>4.4819999999999709</v>
+      </c>
+      <c r="K7" t="s">
         <v>10</v>
       </c>
-      <c r="G7">
+      <c r="L7">
         <f>12</f>
         <v>12</v>
       </c>
-      <c r="H7" t="s">
+      <c r="M7" t="s">
         <v>11</v>
       </c>
-      <c r="I7">
+      <c r="N7">
         <v>15.994915000000001</v>
       </c>
-      <c r="J7" t="s">
+      <c r="O7" t="s">
         <v>12</v>
       </c>
-      <c r="K7">
-        <f>I7*G7/(I7+G7)</f>
+      <c r="P7">
+        <f>N7*L7/(N7+L7)</f>
         <v>6.8562087079028471</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>-20</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>2064.366</v>
       </c>
-      <c r="J8" t="s">
+      <c r="E8">
+        <f>-A8</f>
+        <v>-19</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>4.4490000000000691</v>
+      </c>
+      <c r="O8" t="s">
         <v>13</v>
       </c>
-      <c r="K8">
-        <f>K7/6.022E+23/1000</f>
+      <c r="P8">
+        <f>P7/6.022E+23/1000</f>
         <v>1.1385268528566667E-26</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>-19</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>2068.8150000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f>-A9</f>
+        <v>-18</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>4.4180000000001201</v>
+      </c>
+      <c r="K9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9">
+        <v>2169.81358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>-18</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>2073.2330000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f>-A10</f>
+        <v>-17</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>4.3840000000000146</v>
+      </c>
+      <c r="K10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10">
+        <v>13.288309999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>-17</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>2077.6170000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f>-A11</f>
+        <v>-16</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>4.3519999999998618</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>-16</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>2081.9690000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f>-A12</f>
+        <v>-15</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>4.3200000000001637</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>-15</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>2086.2890000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f>-A13</f>
+        <v>-14</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>4.2859999999996035</v>
+      </c>
+      <c r="I13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" t="e">
+        <f t="array" ref="J13:K13">LINEST(F2:F52,E2:E52)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K13" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>-14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>2090.5749999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f>-A14</f>
+        <v>-13</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>4.2540000000003602</v>
+      </c>
+      <c r="I14" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" s="4" t="e">
+        <f>-J13/2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K14" t="s">
+        <v>43</v>
+      </c>
+      <c r="L14" s="4" t="e">
+        <f>(K13+3*J14)/2</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>-13</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>2094.8290000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f>-A15</f>
+        <v>-12</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>4.2199999999997999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>-12</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>2099.049</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f>-A16</f>
+        <v>-11</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>4.1869999999998981</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>-11</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>2103.2359999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f>-A17</f>
+        <v>-10</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>4.1530000000002474</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>-10</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>2107.3890000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f>-A18</f>
+        <v>-9</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>4.1199999999998909</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>-9</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>2111.509</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <f>-A19</f>
+        <v>-8</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>4.0859999999997854</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>-8</v>
+        <v>7</v>
       </c>
       <c r="B20">
         <v>2115.5949999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f>-A20</f>
+        <v>-7</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>4.0520000000001346</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>-7</v>
+        <v>6</v>
       </c>
       <c r="B21">
         <v>2119.6469999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21">
+        <f>-A21</f>
+        <v>-6</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>4.0180000000000291</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="B22">
         <v>2123.665</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22">
+        <f>-A22</f>
+        <v>-5</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>3.9830000000001746</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>-5</v>
-      </c>
-      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="B23" s="8">
         <v>2127.6480000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23">
+        <f>-A23</f>
+        <v>-4</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>3.9490000000000691</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>-4</v>
-      </c>
-      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="B24" s="9">
         <v>2131.5970000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24">
+        <f>-A24</f>
+        <v>-3</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>3.9149999999999636</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>-3</v>
-      </c>
-      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="B25" s="7">
         <v>2135.5120000000002</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25">
+        <f>-A25</f>
+        <v>-2</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>3.8799999999996544</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="B26">
         <v>2139.3919999999998</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26">
+        <f>-A26</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
       <c r="B28">
         <v>2147.047</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28">
+        <f>A28+1</f>
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>3.7750000000000909</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29">
         <v>2150.8220000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="8">
+        <f>B30-B23</f>
+        <v>26.913000000000011</v>
+      </c>
+      <c r="E29">
+        <f>A29+1</f>
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>3.7390000000000327</v>
+      </c>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="8">
         <v>2154.5610000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="8">
+        <f>D29/4/(3.5)</f>
+        <v>1.9223571428571435</v>
+      </c>
+      <c r="E30">
+        <f>A30+1</f>
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>3.7049999999999272</v>
+      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="9">
         <v>2158.2660000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="4">
+        <f>D30+0.5*D32</f>
+        <v>1.9310714285714343</v>
+      </c>
+      <c r="E31">
+        <f>A31+1</f>
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>3.6680000000001201</v>
+      </c>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4</v>
       </c>
       <c r="B32">
         <v>2161.9340000000002</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="4">
+        <f>D30-D34</f>
+        <v>1.7428571428581563E-2</v>
+      </c>
+      <c r="E32">
+        <f>A32+1</f>
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>3.6329999999998108</v>
+      </c>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>5</v>
       </c>
       <c r="B33">
         <v>2165.567</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="9">
+        <f>B31-B24</f>
+        <v>26.668999999999869</v>
+      </c>
+      <c r="E33">
+        <f>A33+1</f>
+        <v>6</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>3.5970000000002074</v>
+      </c>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>6</v>
       </c>
       <c r="B34">
         <v>2169.1640000000002</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="9">
+        <f>D33/4/(3.5)</f>
+        <v>1.904928571428562</v>
+      </c>
+      <c r="E34">
+        <f>A34+1</f>
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>3.5599999999999454</v>
+      </c>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7</v>
       </c>
       <c r="B35">
         <v>2172.7240000000002</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <f>A35+1</f>
+        <v>8</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>3.5249999999996362</v>
+      </c>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>8</v>
       </c>
       <c r="B36">
         <v>2176.2489999999998</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <f>A36+1</f>
+        <v>9</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>3.4880000000002838</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>9</v>
       </c>
       <c r="B37">
         <v>2179.7370000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <f>A37+1</f>
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>3.4519999999997708</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>10</v>
       </c>
       <c r="B38">
         <v>2183.1889999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <f>A38+1</f>
+        <v>11</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>3.4160000000001673</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>11</v>
       </c>
       <c r="B39">
         <v>2186.605</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <f>A39+1</f>
+        <v>12</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>3.3780000000001564</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>12</v>
       </c>
       <c r="B40">
         <v>2189.9830000000002</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <f>A40+1</f>
+        <v>13</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>3.3419999999996435</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>13</v>
       </c>
       <c r="B41">
         <v>2193.3249999999998</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <f>A41+1</f>
+        <v>14</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>3.3040000000000873</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>14</v>
       </c>
       <c r="B42">
         <v>2196.6289999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <f>A42+1</f>
+        <v>15</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>3.2670000000002801</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>15</v>
       </c>
       <c r="B43">
         <v>2199.8960000000002</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <f>A43+1</f>
+        <v>16</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>3.2300000000000182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>16</v>
       </c>
       <c r="B44">
         <v>2203.1260000000002</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <f>A44+1</f>
+        <v>17</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>3.1929999999997563</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>17</v>
       </c>
       <c r="B45">
         <v>2206.319</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <f>A45+1</f>
+        <v>18</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>3.1550000000002001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>18</v>
       </c>
       <c r="B46">
         <v>2209.4740000000002</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <f>A46+1</f>
+        <v>19</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>3.1169999999997344</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>19</v>
       </c>
       <c r="B47">
         <v>2212.5909999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <f>A47+1</f>
+        <v>20</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>3.0790000000001783</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>20</v>
       </c>
       <c r="B48">
         <v>2215.67</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <f>A48+1</f>
+        <v>21</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>3.0409999999997126</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>21</v>
       </c>
       <c r="B49">
         <v>2218.7109999999998</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <f>A49+1</f>
+        <v>22</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>3.0030000000001564</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>22</v>
       </c>
       <c r="B50">
         <v>2221.7139999999999</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <f>A50+1</f>
+        <v>23</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>2.9650000000001455</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>23</v>
       </c>
       <c r="B51">
         <v>2224.6790000000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <f>A51+1</f>
+        <v>24</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>2.9259999999999309</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>24</v>
       </c>
       <c r="B52">
         <v>2227.605</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <f>A52+1</f>
+        <v>25</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>2.88799999999992</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>25</v>
       </c>
       <c r="B53">
         <v>2230.4929999999999</v>
       </c>
+      <c r="E53">
+        <f>A53+1</f>
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5502,14 +8472,14 @@
   <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5517,7 +8487,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>-26</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>1945.9</v>
@@ -5525,7 +8495,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>-25</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>1954.309</v>
@@ -5533,7 +8503,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>-24</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>1962.69</v>
@@ -5541,7 +8511,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>-23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>1971.0429999999999</v>
@@ -5549,7 +8519,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>-22</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>1979.367</v>
@@ -5557,7 +8527,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>-21</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>1987.663</v>
@@ -5565,7 +8535,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>-20</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>1995.9290000000001</v>
@@ -5573,7 +8543,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>-19</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>2004.1659999999999</v>
@@ -5581,7 +8551,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>-18</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>2012.373</v>
@@ -5589,7 +8559,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>-17</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>2020.55</v>
@@ -5597,7 +8567,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>-16</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>2028.6969999999999</v>
@@ -5605,7 +8575,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>-15</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>20363812</v>
@@ -5613,7 +8583,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>-14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>2044.8969999999999</v>
@@ -5621,7 +8591,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>-13</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>2052.951</v>
@@ -5629,7 +8599,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>-12</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>2060.973</v>
@@ -5637,7 +8607,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>-11</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>2068.9630000000002</v>
@@ -5645,7 +8615,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>-10</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>2076.922</v>
@@ -5653,7 +8623,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>-9</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>2084.8470000000002</v>
@@ -5661,7 +8631,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>-8</v>
+        <v>7</v>
       </c>
       <c r="B20">
         <v>2092.7399999999998</v>
@@ -5669,7 +8639,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>-7</v>
+        <v>6</v>
       </c>
       <c r="B21">
         <v>2100.6</v>
@@ -5677,7 +8647,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>-6</v>
+        <v>5</v>
       </c>
       <c r="B22">
         <v>2108.4259999999999</v>
@@ -5685,7 +8655,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>-5</v>
+        <v>4</v>
       </c>
       <c r="B23">
         <v>2116.2190000000001</v>
@@ -5693,7 +8663,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>-4</v>
+        <v>3</v>
       </c>
       <c r="B24">
         <v>2123.9780000000001</v>
@@ -5701,7 +8671,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="B25">
         <v>2131.7020000000002</v>
@@ -5918,4 +8888,447 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A1310E6-49B2-4544-930D-A3D372686A01}">
+  <dimension ref="A1:U17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>A2+0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>$I$9-2*(A2+1)*$I$10</f>
+        <v>2143.2369600000002</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B14" si="0">A3+0.5</f>
+        <v>1.5</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C14" si="1">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D14" si="2">$I$9-2*(A3+1)*$I$10</f>
+        <v>2116.6603399999999</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <f>1.93128-0.5*0.01750441</f>
+        <v>1.9225277950000002</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3">
+        <v>1.128323</v>
+      </c>
+      <c r="O3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3">
+        <v>0.5</v>
+      </c>
+      <c r="Q3">
+        <f>D2</f>
+        <v>2143.2369600000002</v>
+      </c>
+      <c r="S3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T3" s="4">
+        <f>(Q4-Q3)/(P4-P3)</f>
+        <v>-26.576620000000009</v>
+      </c>
+      <c r="U3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>2090.0837200000001</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4">
+        <v>6.1878000000000003E-6</v>
+      </c>
+      <c r="O4" t="s">
+        <v>49</v>
+      </c>
+      <c r="P4">
+        <v>12.5</v>
+      </c>
+      <c r="Q4">
+        <f>D14</f>
+        <v>1824.3175200000001</v>
+      </c>
+      <c r="S4" t="s">
+        <v>51</v>
+      </c>
+      <c r="T4">
+        <f>Q3-P3*T3</f>
+        <v>2156.5252700000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>2063.5070999999998</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5">
+        <v>1.9050229999999999</v>
+      </c>
+      <c r="S5" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5">
+        <f>-T4/T3</f>
+        <v>81.143699612667049</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>2036.93048</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6">
+        <v>6.1724999999999998E-6</v>
+      </c>
+      <c r="S6" t="s">
+        <v>55</v>
+      </c>
+      <c r="T6" s="4">
+        <f>-0.5*T3+T4</f>
+        <v>2169.81358</v>
+      </c>
+      <c r="U6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>2010.3538599999999</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="J7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7">
+        <v>15.994915000000001</v>
+      </c>
+      <c r="L7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <f>K7*I7/(K7+I7)</f>
+        <v>6.8562087079028471</v>
+      </c>
+      <c r="S7" t="s">
+        <v>20</v>
+      </c>
+      <c r="T7" s="4">
+        <f>0.5*T3*T5^2+T4*T5</f>
+        <v>87494.219358002854</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <f>$I$9-2*(A8+1)*$I$10</f>
+        <v>1983.7772399999999</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8">
+        <f>M7/6.022E+23/1000</f>
+        <v>1.1385268528566667E-26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>1957.2006200000001</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9">
+        <v>2169.81358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>1930.624</v>
+      </c>
+      <c r="H10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10">
+        <v>13.288309999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>1904.04738</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>10.5</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>1877.4707600000002</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>1850.8941399999999</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13">
+        <f t="array" ref="F13:G13">LINEST(D2:D14,B2:B14)</f>
+        <v>-26.576620000000002</v>
+      </c>
+      <c r="G13">
+        <v>2156.5252700000001</v>
+      </c>
+      <c r="H13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>1824.3175200000001</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14">
+        <f>-G13/F13</f>
+        <v>81.143699612667078</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="4">
+        <f>0.5*F13*G14^2+G13*G14</f>
+        <v>87494.219358002883</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="array" ref="F17:G17">LINEST(D2:D14,C2:C14)</f>
+        <v>-26.576620000000002</v>
+      </c>
+      <c r="G17" s="4">
+        <v>2169.81358</v>
+      </c>
+      <c r="H17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update the quiz spectra spreadsheet
</commit_message>
<xml_diff>
--- a/Quizzes/Spectra.xlsx
+++ b/Quizzes/Spectra.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthewrowley1\Desktop\3620\Quizzes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468AC43C-74F6-424D-866A-AF9408C0F817}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E61DA1-EFC2-4867-A9D8-F17E263BD429}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{E65C0530-7A76-4299-804D-8365C5750414}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="6" xr2:uid="{E65C0530-7A76-4299-804D-8365C5750414}"/>
   </bookViews>
   <sheets>
     <sheet name="CN Microwave" sheetId="11" r:id="rId1"/>
@@ -267,7 +267,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,6 +310,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -323,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -335,6 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5064,6 +5071,9 @@
                 <c:pt idx="24">
                   <c:v>-1</c:v>
                 </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="26">
                   <c:v>1</c:v>
                 </c:pt>
@@ -5222,6 +5232,12 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>3.8799999999996544</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.8450425563355566</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.8099574436646435</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>3.7750000000000909</c:v>
@@ -11386,15 +11402,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
+      <xdr:colOff>323849</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:rowOff>90486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13032,7 +13048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19142631-294F-494D-9269-3DFAB8A4A463}">
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -16943,8 +16959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535BBEDA-FF49-4A25-AA6B-6D84D95D0A37}">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="D12" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17321,6 +17337,10 @@
         <f t="shared" si="3"/>
         <v>4.3200000000001637</v>
       </c>
+      <c r="N12">
+        <f>J13*-1+K13</f>
+        <v>3.8283851126708486</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -17357,6 +17377,9 @@
       </c>
       <c r="L13" t="s">
         <v>36</v>
+      </c>
+      <c r="M13">
+        <v>3.7933300000000001</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -17600,7 +17623,10 @@
       <c r="B23" s="7">
         <v>2127.6480000000001</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="C23" s="6">
+        <f>AVERAGE(C25:C26)</f>
+        <v>2143.2370425563354</v>
+      </c>
       <c r="D23" s="6"/>
       <c r="E23">
         <f t="shared" si="0"/>
@@ -17652,7 +17678,10 @@
       <c r="B25" s="6">
         <v>2135.5120000000002</v>
       </c>
-      <c r="C25" s="6"/>
+      <c r="C25" s="6">
+        <f>B26+N12</f>
+        <v>2143.2203851126706</v>
+      </c>
       <c r="D25" s="6"/>
       <c r="E25">
         <f t="shared" si="0"/>
@@ -17678,12 +17707,19 @@
       <c r="B26">
         <v>2139.3919999999998</v>
       </c>
-      <c r="C26" s="6"/>
+      <c r="C26" s="6">
+        <f>B28-3.7933</f>
+        <v>2143.2537000000002</v>
+      </c>
       <c r="D26" s="6"/>
       <c r="E26">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
+      <c r="F26" s="11">
+        <f t="shared" si="1"/>
+        <v>3.8450425563355566</v>
+      </c>
       <c r="G26">
         <f>E28</f>
         <v>1</v>
@@ -17694,8 +17730,19 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="11">
+        <f>C23</f>
+        <v>2143.2370425563354</v>
+      </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="11">
+        <f t="shared" si="1"/>
+        <v>3.8099574436646435</v>
+      </c>
       <c r="G27">
         <f t="shared" ref="G27:H27" si="4">E29</f>
         <v>2</v>

</xml_diff>